<commit_message>
updated charts added perf-power-charts
</commit_message>
<xml_diff>
--- a/Ranking/Rankings.xlsx
+++ b/Ranking/Rankings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\BrsVgl\PerformanceEfficiencySuite.PS\Ranking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F28B9F-2665-4FB9-83C6-ADF35FD7FF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6529D3AB-A391-4BE5-A655-17FF8684C476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="693" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8437,7 +8437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F06E1893-BD0F-4CAA-8A26-DF7FF54A2AFD}" type="CELLRANGE">
+                    <a:fld id="{F58A9B6F-7B7B-4469-96C0-52B41B6674F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8470,7 +8470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70619ED5-7951-4C84-800E-D48CCC78907B}" type="CELLRANGE">
+                    <a:fld id="{D0A3FCB0-DF78-4D3A-9A7A-A8FE2CCD73BF}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8504,7 +8504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B5170AA-F223-4D6D-AC6E-345C5807CB1C}" type="CELLRANGE">
+                    <a:fld id="{8331B24C-24E8-47CA-88F3-CF3641291E2C}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8572,7 +8572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0526B101-91C1-4981-8E19-A3C37FC96C9B}" type="CELLRANGE">
+                    <a:fld id="{B65A9DEC-7C33-4604-8EB8-A75F2DDBED1F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8639,7 +8639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6F97964-3BC5-4C97-9465-1F6A8BEEF7FC}" type="CELLRANGE">
+                    <a:fld id="{9C1B6239-F407-489E-B61F-E3E603720508}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8756,7 +8756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC99EA03-1A43-4380-B02D-A9B1E2156E7B}" type="CELLRANGE">
+                    <a:fld id="{6D2D8931-8235-46F1-8017-1DFB0E95365B}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8796,7 +8796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D35BA250-5FFF-41EC-A540-60499A051AC2}" type="CELLRANGE">
+                    <a:fld id="{33D87645-0B92-4DFA-AC36-6F5A9B8514D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -8941,7 +8941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C77190B1-A6B5-4D6F-A7B6-F075AEC7934A}" type="CELLRANGE">
+                    <a:fld id="{0C7A4DF8-4371-48F2-B65B-9BB278DA916C}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9115,7 +9115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{752674AA-9DA9-4B15-A9A8-ABF4CA245992}" type="CELLRANGE">
+                    <a:fld id="{5A2DD29E-F84D-4115-90EE-BDF7EC504ED5}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9261,7 +9261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD1E6C61-25F4-4954-BC36-330EC38254F4}" type="CELLRANGE">
+                    <a:fld id="{19308448-306E-48A2-B649-9155A9ED649F}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9329,7 +9329,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF0995AE-AC13-4087-892A-BA6796D216F2}" type="CELLRANGE">
+                    <a:fld id="{C8B323B9-C2E5-4490-8B3C-86782194F978}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9390,7 +9390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{00E97D8B-E38F-4F6F-9F2C-4A6A73377504}" type="CELLRANGE">
+                    <a:fld id="{31B37857-D519-4953-933C-95C21E9444FD}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9452,7 +9452,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFEB88FB-B285-4B0B-A674-BE02E5792195}" type="CELLRANGE">
+                    <a:fld id="{5A39B0FA-11CB-4CAB-B12A-68937B416395}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9514,7 +9514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88CE5F43-8113-4886-AB3A-66878C4211CA}" type="CELLRANGE">
+                    <a:fld id="{7FE93A9E-82EE-4D99-85B3-E09C8BAC1F1A}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9548,7 +9548,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9B0DE6F-BE1C-4E21-B150-D04EDCAA9718}" type="CELLRANGE">
+                    <a:fld id="{4F741B4E-BA0E-4561-AD84-8D5A5E2D11B6}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9610,7 +9610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A9DEC10-EEEC-49E1-8940-3FEF39505414}" type="CELLRANGE">
+                    <a:fld id="{F20BA2DD-C52D-4F6D-9968-D30C463ABBB9}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9650,7 +9650,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4EB53BD-8CFC-411A-8A9A-855F2B38739F}" type="CELLRANGE">
+                    <a:fld id="{82374E4E-5DDA-4DB7-B990-A3F84EC65961}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9683,7 +9683,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F98C752-1019-4FAC-8E1D-1F71DD9BBC23}" type="CELLRANGE">
+                    <a:fld id="{EBCE86E8-5612-4D2A-8297-841B12BF835F}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9745,7 +9745,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D60AD9EE-4BB6-4E98-86A7-1DC98E46666D}" type="CELLRANGE">
+                    <a:fld id="{423938CC-F5BB-4720-BB4C-42EAE3C607D0}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9779,7 +9779,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E2A49940-255A-4CFE-AE6C-5628A397C262}" type="CELLRANGE">
+                    <a:fld id="{23390592-19BF-48A6-9BE7-A7B89ACDE41F}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9869,7 +9869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36546854-C711-4F9C-A16B-F5F05D6C0E12}" type="CELLRANGE">
+                    <a:fld id="{53642E9C-3AC9-4734-B2E0-3EFF776B28D0}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -9987,7 +9987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{740F12D4-EEBD-4563-9482-BEFB3D8CFF10}" type="CELLRANGE">
+                    <a:fld id="{AFBCA4C7-2EDE-442F-8EB7-14D2F59E5BCD}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10027,7 +10027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8864414-1C1C-49D9-B075-58D0371A3835}" type="CELLRANGE">
+                    <a:fld id="{61A14568-5F99-48B3-9776-A1E99E2F4495}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10116,7 +10116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCAB4233-D42E-49FA-8A66-C95B98457D67}" type="CELLRANGE">
+                    <a:fld id="{2134EB39-9322-4635-864C-49BE16B1BD43}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10150,7 +10150,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60647064-A6A0-43F8-BFFF-6E76C821140D}" type="CELLRANGE">
+                    <a:fld id="{3CA517CD-D043-4062-A6E8-8B1829A8F7A5}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10184,7 +10184,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF12EEB1-9410-454F-A238-17385E9E6609}" type="CELLRANGE">
+                    <a:fld id="{E51F2F8D-8E73-4512-B2EC-437FAAC0FC72}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10218,7 +10218,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CBAFB4C-18C7-46AE-A084-272ECA95C5C1}" type="CELLRANGE">
+                    <a:fld id="{C4F707D4-F468-4920-81AB-05463866E1CE}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10280,7 +10280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F009F6C-9741-4C3E-8BEE-C0CC55DC9645}" type="CELLRANGE">
+                    <a:fld id="{690C0309-914C-4298-ADDB-944847191DA8}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10314,7 +10314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3459E930-9A4F-4218-BB57-42DBACC61BBF}" type="CELLRANGE">
+                    <a:fld id="{3759D2CC-32B7-44C1-A0BF-1431D23A81A5}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10410,7 +10410,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE492215-3975-416E-AE6F-268C4BE5D937}" type="CELLRANGE">
+                    <a:fld id="{5A7F7973-C50A-489D-95D8-463C36F61855}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10477,7 +10477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CF44290-769F-4454-A76F-37D1C7827300}" type="CELLRANGE">
+                    <a:fld id="{7E528F9E-0E14-46A8-8C54-93A2E852531D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10566,7 +10566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A031E2D3-1D85-42E5-B282-572F344793D9}" type="CELLRANGE">
+                    <a:fld id="{49D666FD-CD4A-4570-A640-E22B9ABC23B9}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10600,7 +10600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31724A6F-24AA-433A-B626-2F5631074529}" type="CELLRANGE">
+                    <a:fld id="{44B84F73-0BE8-41EE-A773-A7902CEEB814}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10634,7 +10634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC9E17AA-8D28-4FEB-97A0-77605C578180}" type="CELLRANGE">
+                    <a:fld id="{2C4E9FDF-7E2E-48CC-97EC-432EB32E67E6}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10668,7 +10668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEB262FA-43D9-40B9-96E2-34E91D46246E}" type="CELLRANGE">
+                    <a:fld id="{7D47B612-86AB-4F62-AD76-F3AD249EF110}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10702,7 +10702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1340E9B1-2E40-4287-904F-8A68DD0BC033}" type="CELLRANGE">
+                    <a:fld id="{518B8239-5EE3-4080-832D-D00A47E8E1F4}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10736,7 +10736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DEFBC6E-32EA-4800-A1A5-6CB6BDFE0123}" type="CELLRANGE">
+                    <a:fld id="{E03C72D6-E701-4352-A401-EE924D5AFB60}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10776,7 +10776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE2B91B0-8573-4C90-B129-0DF23C7CA5AA}" type="CELLRANGE">
+                    <a:fld id="{F13C69AF-099C-4383-84F5-3F0D27C662BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10837,7 +10837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3329380E-D1B0-4E0A-B6DE-6EB416853BBD}" type="CELLRANGE">
+                    <a:fld id="{525B20CB-EA1B-4457-BB58-09FE4666EEE9}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10871,7 +10871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E4BADA53-3B06-4778-AADE-5A1E9A4BDD84}" type="CELLRANGE">
+                    <a:fld id="{8DCFCA6B-3B4D-4C60-9E1F-A19CC24BFC10}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10905,7 +10905,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C1503B1-084C-42E0-9D02-231569DDD617}" type="CELLRANGE">
+                    <a:fld id="{731AED43-241E-42E4-A651-F4C98364EE68}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10945,7 +10945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F17E57E-9116-4440-98F9-62DF16713495}" type="CELLRANGE">
+                    <a:fld id="{AC56F2F6-CE4C-4393-B0C9-67DBEE81A5A9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -10984,7 +10984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1385357-40AB-460D-93AE-FB38919829EF}" type="CELLRANGE">
+                    <a:fld id="{23BF368A-CE53-45F7-96A6-13B1493C5C34}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -11023,7 +11023,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF3122F8-7942-4F08-B330-FFCB4CEE99BA}" type="CELLRANGE">
+                    <a:fld id="{93DEAFFE-B5E9-41D4-B4D9-475140085D17}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -11056,7 +11056,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30BBAA31-053E-4D78-B65C-A36DC4CEFADF}" type="CELLRANGE">
+                    <a:fld id="{EA18061B-3D9B-4F1A-B38A-8295270812F9}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -11118,7 +11118,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A289424C-BDEE-4117-B00A-B55BC81DE1FF}" type="CELLRANGE">
+                    <a:fld id="{8F40DD5B-5B58-4DED-835E-9D8EF3667AB2}" type="CELLRANGE">
                       <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -11320,8 +11320,8 @@
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
+                          <a:lumMod val="25000"/>
+                          <a:lumOff val="75000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:round/>
@@ -12189,12 +12189,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -12303,12 +12314,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -12371,12 +12393,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -15301,7 +15318,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6EBEC2AD-FA5D-417D-A35C-132FAC5F5776}" type="CELLRANGE">
+                    <a:fld id="{0C84F730-ED18-4087-B645-1AC81705E9A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -15333,8 +15350,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0378E20-619D-4D23-ACC5-3754D8CF2772}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7A3E7BE2-C0C3-41C7-A8B4-384541886259}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -15351,6 +15368,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -15365,8 +15383,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8116B91-84AA-4AAB-A4A9-7137CC0E25B8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{CA003703-878D-4C63-B8CB-CC595B5F724F}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -15383,6 +15401,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -15430,7 +15449,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{040856A4-FCAE-42BE-A4EB-B7D4D830B5EE}" type="CELLRANGE">
+                    <a:fld id="{0211FB29-9AC8-4814-9D62-27F3C79EF4CF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -15495,7 +15514,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E25135F0-C058-4A6A-B29E-CD96375727A4}" type="CELLRANGE">
+                    <a:fld id="{2E5D49EC-C8FC-45A3-8FA4-73C9104DA203}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -15608,8 +15627,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7680D7E-A94A-4954-8181-F8A6E576F8A0}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{62451703-622E-4A76-8B16-59A0A73DC4CD}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -15626,6 +15645,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -15640,8 +15660,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC63BA58-F579-4687-B39A-69B98B7771B5}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4026A46D-BB77-4511-B64D-7B56539DB271}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -15658,6 +15678,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -15786,7 +15807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9206F032-0617-4522-A470-67074E6DDDEB}" type="CELLRANGE">
+                    <a:fld id="{6E1E0525-F050-4BAA-A7CC-9E980BB7C2C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -15953,8 +15974,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DD6C054-F80F-4DDE-A42E-A5DA31EB3706}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{A6722907-2CD7-4E14-933F-BED875A24D40}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -15971,6 +15992,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16093,8 +16115,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D45F4B9-933A-4FDC-9915-2ED3745F402B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{59DCC3B4-CA71-47CD-9A05-D83305FB1C12}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16111,6 +16133,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16152,8 +16175,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35333055-950D-4652-98AD-3158E9953089}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{C1B619BC-B6A3-420B-B6C3-D68FA19ED5A0}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16170,6 +16193,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16211,8 +16235,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47838756-00AA-4208-91EA-D3CC5A2AD052}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F6B4E16B-844E-4A17-AC42-F1EBBAE8E856}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16229,6 +16253,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16270,8 +16295,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D271ACA-807F-4734-B179-7421F7B2C7C5}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4584A3E4-2A05-4338-B327-C892831BC99B}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16288,6 +16313,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16329,8 +16355,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F607856C-03A6-4001-A7BD-570CB111DA3B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{8D19BE18-BACB-40FE-B23F-2A59F37D7379}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16347,6 +16373,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16361,8 +16388,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45BD63FD-6412-483B-A4B0-355369D0D8ED}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{CF4E4F97-A848-45A0-9EBC-F5A45E47A627}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16379,6 +16406,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16426,7 +16454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCC0E20F-CA5D-4E74-9517-50101ED83789}" type="CELLRANGE">
+                    <a:fld id="{198886A9-05AB-45A8-8600-7BB9D49A1345}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -16458,8 +16486,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A31E9C3-52BD-40DC-9D0C-E70444EEE899}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{07876B4B-FBEB-49B9-B9DD-A5E49CC72912}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16476,6 +16504,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16490,8 +16519,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A75AB457-B805-4E44-BCDC-989D452B9450}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{5B4A78C0-AE41-426D-86FE-8D31AD28DF6C}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16508,6 +16537,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16549,8 +16579,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F4FBC52-9B4F-4B1E-8AE6-2FDA0517875E}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{CEACA2C7-097F-42F0-810F-2C092E934EF2}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16567,6 +16597,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16581,8 +16612,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A83B3F75-493F-4AD8-8468-A4BCAC7B396A}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{3F1C08D7-9C5B-4003-A830-3378FE65CA4C}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16599,6 +16630,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16673,7 +16705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A39CF4AA-18E6-4B46-B375-F91E3DD2D344}" type="CELLRANGE">
+                    <a:fld id="{16E94B8F-D269-4688-A178-9DF66541C42F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -16786,8 +16818,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1229FCF-FAD5-442C-90DF-7E9CF1AE6309}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{1E289920-90D4-454F-8C22-A07AB0839715}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16804,6 +16836,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16818,8 +16851,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A308EF5A-AF79-4CC2-8C23-4ABAE58B6D0E}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{AFD72AD8-0F70-443C-9E80-9C79C56BE8BF}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16836,6 +16869,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16904,8 +16938,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBBF9656-0449-4B97-B6DF-B336103C72C1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{911DD4C5-72E1-487E-AD12-FBE5137AA9EC}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16922,6 +16956,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16936,8 +16971,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E74D7651-2F67-4229-9AFE-494E186381E7}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0D1E2799-5FED-450C-ABF4-3B645F6C087B}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -16954,6 +16989,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -16974,7 +17010,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A6F69A0-1FD2-4818-A9F6-FDCEE9FEBA38}" type="CELLRANGE">
+                    <a:fld id="{7F9B34F6-AEF7-4D97-8B4C-23C23595562E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -17006,8 +17042,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{999CBDE4-CD34-4C24-865C-37318FF71BA7}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{93725383-12FB-4760-BAF7-96CCED3073D8}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17024,6 +17060,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17065,8 +17102,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F2C8222-4514-46AE-9A2B-746441AB80A6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{01C99215-8B44-413A-906F-F606A597CE48}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17083,6 +17120,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17097,8 +17135,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15836EB0-B503-451D-9A76-623EC799A517}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{86360672-4176-48B6-BD95-154F8BDEDFE6}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17115,6 +17153,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17189,7 +17228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69B97024-4D1A-4EAF-B01A-02A672F2C8FF}" type="CELLRANGE">
+                    <a:fld id="{DF103D62-9EB9-429C-85FA-BB1C7C453884}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -17248,8 +17287,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB233D86-3915-4A84-8067-68138B42FC3A}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{89C493B2-6D9F-41EC-9023-7D5C16AC5C1B}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17266,6 +17305,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17334,8 +17374,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E3E718D7-804B-4167-BD8A-4C8BFFFCBEB3}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0D322ED9-D25A-489F-9DD6-3630E82C37FB}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17352,6 +17392,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17366,8 +17407,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB9EAE5D-BE15-4AA2-B2D7-84A4CD8F2CEB}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{FD945E38-706B-4576-950A-DEA4E26490C6}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17384,6 +17425,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17398,8 +17440,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB08D102-F477-4E05-B0FD-66AE4CCE6473}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F85FBFD5-14C9-41A2-8A2F-7CD837C1EEE4}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17416,6 +17458,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17430,8 +17473,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A179598-296B-4B9E-8036-4010D4D9EA01}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0FBD45CC-27A4-4091-B6F5-20F3D0F42E7E}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17448,6 +17491,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17462,8 +17506,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CF5ED06-EE76-42D6-9221-D18E36D647BA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{94ECDB6B-38B8-45B4-B3E7-EADFB9B80D19}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17480,6 +17524,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17494,8 +17539,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D491F0D2-DE50-4FA1-82FA-9A991C09AD84}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{34C224CB-3173-4CF6-B960-71656E0862D7}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17512,6 +17557,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17526,8 +17572,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4194276B-6E29-4B62-BA8D-47A53C45E445}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9A9C625A-D744-4D93-8B8F-298D5E044D28}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17544,6 +17590,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17585,8 +17632,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EA3A9C9-0AC1-4A59-8873-B4B8CED87968}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2EEBEA71-EA63-41E5-B82D-F74E7C323839}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17603,6 +17650,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17617,8 +17665,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E134F10-B50D-4E16-85C0-FBED67536F21}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{BFBF8C2B-CC99-47A9-A110-916B2FA1960C}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17635,6 +17683,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17649,8 +17698,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E020704A-E4B6-4229-BDAB-FAAE7E9038D3}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{23CD89C3-8B4E-43CA-9276-AE87FC13CA8D}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17667,6 +17716,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17681,8 +17731,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A33E84E-0233-4432-A763-D588EC008FB4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{BF58F274-DC53-47B3-9745-8A07307AB423}" type="CELLRANGE">
+                      <a:rPr lang="de-DE"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
                     </a:fld>
@@ -17699,6 +17749,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -17719,7 +17770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17B42555-E455-4F36-83B2-790D6AE6EEB9}" type="CELLRANGE">
+                    <a:fld id="{2EAA89E0-3E2F-4062-9218-EBE6C66CE885}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -17757,7 +17808,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77033FF0-3AC6-4F6C-9BAA-CCEC5E36E6B8}" type="CELLRANGE">
+                    <a:fld id="{0C08DA78-098F-4111-8928-B4C2D51C8100}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -17795,7 +17846,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4955AA20-FA68-4E75-B161-40C820D5750C}" type="CELLRANGE">
+                    <a:fld id="{AD225F3E-9784-477C-86D8-098D25273BAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -17860,7 +17911,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6A0BB671-E3A7-402A-BB4C-52E28C4B5295}" type="CELLRANGE">
+                    <a:fld id="{539C6C5F-7D8B-4360-8389-2507B7E79CB5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[ZELLBEREICH]</a:t>
@@ -18907,7 +18958,9 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -19021,7 +19074,9 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -22645,14 +22700,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>716280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180473</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>206520</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>36473</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24849,7 +24904,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FC0BFEFE-A716-4026-A564-144290A7DD0A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="37">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FC0BFEFE-A716-4026-A564-144290A7DD0A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="39">
   <location ref="B3:C51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -25221,7 +25276,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{056CE95F-2CE7-42FD-BB6D-DBBA62D051FD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="34">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{056CE95F-2CE7-42FD-BB6D-DBBA62D051FD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="36">
   <location ref="B3:C51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -25593,7 +25648,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9BB96FF-3D68-4286-89DF-310DCD70893C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="36">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B9BB96FF-3D68-4286-89DF-310DCD70893C}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="38">
   <location ref="B3:C51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -25965,7 +26020,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81875018-2FDD-4D02-B5CA-D328CB30719D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="40">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{81875018-2FDD-4D02-B5CA-D328CB30719D}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="42">
   <location ref="B3:C51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -26313,7 +26368,7 @@
   <dataFields count="1">
     <dataField name="Summe von Cons. MT" fld="14" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="11">
+  <chartFormats count="13">
     <chartFormat chart="4" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -26405,6 +26460,24 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="39" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="40" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="41" format="11" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -26774,7 +26847,7 @@
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J91" sqref="J91"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -33875,8 +33948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{093893EB-1C3B-4AC4-A954-F4CE9F9B9C4A}">
   <dimension ref="B4:F93"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="S38" sqref="S38"/>
+    <sheetView topLeftCell="F17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35609,8 +35682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A2D50E-9363-488B-9BFC-B64ADDEEA2B0}">
   <dimension ref="B4:F93"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="D31" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>